<commit_message>
Fixed all tests, added copy method to Arithmetic_Dict
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pleba\Desktop\konc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D27318D-51B9-4B12-A87C-D1467A3B9B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E46C7F-8B69-45CC-9EB3-585B8CEA7DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E4D1C54E-4B6D-4636-B891-302CDD2D5CBD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>food</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>tools</t>
-  </si>
-  <si>
-    <t>avalilable</t>
   </si>
   <si>
     <t>needed</t>
@@ -617,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAE5964-51D9-4F83-BE49-7B6E99C5E897}">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="P31" sqref="B31:P31"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,7 +627,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -704,7 +701,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="5">
         <v>100</v>
@@ -752,10 +749,10 @@
         <v>50</v>
       </c>
       <c r="Q3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>5</v>
       </c>
       <c r="S3" s="6">
         <f>SUM(B3:P3)</f>
@@ -764,7 +761,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
         <v>50</v>
@@ -813,7 +810,7 @@
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S4" s="6">
         <f>SUM(B4:P4)</f>
@@ -822,7 +819,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <f>SUM(B3,G3,L3)</f>
@@ -860,7 +857,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5">
         <f>SUM(B4,G4,L4)</f>
@@ -898,7 +895,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="10">
         <v>1</v>
@@ -931,7 +928,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="5">
         <f>B6*B7/B5</f>
@@ -969,7 +966,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="5">
         <f>MIN(IF(B8=0,1E+40,B4/B8),B4)</f>
@@ -1058,7 +1055,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5">
         <f>$B$8*B3</f>
@@ -1126,7 +1123,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="5">
         <f>$B$8*B9</f>
@@ -1194,7 +1191,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="5">
         <f>SUM(B11:F11)</f>
@@ -1226,7 +1223,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5">
         <f>SUM(B12:F12)</f>
@@ -1258,7 +1255,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="5">
         <f>IF(B13&gt;B14,1,0)</f>
@@ -1311,7 +1308,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5">
         <f>$B$15*B9</f>
@@ -1379,7 +1376,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="5">
         <f>(1-B15)*B13/B14</f>
@@ -1411,7 +1408,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="5">
         <f>$B$18*B9</f>
@@ -1479,7 +1476,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5">
         <f>B19+B17</f>
@@ -1568,7 +1565,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1591,7 +1588,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1614,7 +1611,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="5">
         <f t="shared" ref="B24:P24" si="9">B20</f>
@@ -1682,7 +1679,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="5">
         <f>B5-B24-G24-L24</f>
@@ -1720,7 +1717,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="5">
         <f>MAX(B13-B14, 0)</f>
@@ -1735,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F26" s="5">
         <f>SUM(B26:D26)</f>
@@ -1757,7 +1754,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="5">
         <f>B26/$F$26</f>
@@ -1810,7 +1807,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="5">
         <f>B25*$B$27</f>
@@ -1899,7 +1896,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="14">
         <f>B24+B29</f>
@@ -1976,7 +1973,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1987,7 +1984,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1998,15 +1995,15 @@
         <v>1</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="11">
         <v>1</v>
@@ -2023,7 +2020,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="12">
         <v>1.8</v>
@@ -2033,23 +2030,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
+      <c r="A5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="C5" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <f>B5/B4</f>
-        <v>0.55555555555555558</v>
+        <v>0.83333333333333326</v>
       </c>
       <c r="C6">
         <f>C5/C4</f>
@@ -2058,42 +2055,42 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <f>C6/(B6+C6)</f>
-        <v>0.54545454545454541</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <f>F3-C8</f>
-        <v>27.272727272727273</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="C8">
         <f>F3*C7</f>
-        <v>32.727272727272727</v>
+        <v>26.666666666666664</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <f>B8*B3</f>
-        <v>27.272727272727273</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="C9">
         <f>C8*C3</f>
-        <v>49.090909090909093</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10">
         <f>D3*F3</f>
@@ -2102,7 +2099,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2113,15 +2110,15 @@
         <v>1</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="11">
         <v>7.1</v>
@@ -2138,7 +2135,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="12">
         <v>1.8</v>
@@ -2148,67 +2145,67 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
+      <c r="A16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="C16" s="11">
+        <v>1.7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17">
         <f>B16/B15</f>
-        <v>0.55555555555555558</v>
+        <v>0.83333333333333326</v>
       </c>
       <c r="C17">
         <f>C16/C15</f>
-        <v>0.66666666666666663</v>
+        <v>1.1333333333333333</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18">
         <f>C17/(B17+C17)</f>
-        <v>0.54545454545454541</v>
+        <v>0.57627118644067798</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <f>F14-C19</f>
-        <v>27.272727272727273</v>
+        <v>25.423728813559322</v>
       </c>
       <c r="C19">
         <f>F14*C18</f>
-        <v>32.727272727272727</v>
+        <v>34.576271186440678</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <f>B19*B14</f>
-        <v>193.63636363636363</v>
+        <v>180.50847457627117</v>
       </c>
       <c r="C20">
         <f>C19*C14</f>
-        <v>49.090909090909093</v>
+        <v>51.864406779661017</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21">
         <f>D14*F14</f>
@@ -2221,12 +2218,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2344,15 +2338,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D904AF-352E-4CDF-B047-9525628BC63A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{356D2B18-87B5-4836-ACC7-8887E858DF72}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2374,16 +2378,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{356D2B18-87B5-4836-ACC7-8887E858DF72}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D904AF-352E-4CDF-B047-9525628BC63A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tested base methods of State_Data
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pleba\Desktop\konc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0F1E3E-027C-4247-BD62-06EFD1D1E67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F28ACDD-99B4-426F-A73A-47A946FDFAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4D1C54E-4B6D-4636-B891-302CDD2D5CBD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E4D1C54E-4B6D-4636-B891-302CDD2D5CBD}"/>
   </bookViews>
   <sheets>
     <sheet name="test_market.do_trade" sheetId="1" r:id="rId1"/>
     <sheet name="test_market.set_prices" sheetId="3" r:id="rId2"/>
-    <sheet name="test_peasants" sheetId="2" r:id="rId3"/>
+    <sheet name="test_state_data.employ" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="76">
   <si>
     <t>food</t>
   </si>
@@ -120,67 +120,151 @@
     <t>TEST test_market.do_trade()</t>
   </si>
   <si>
-    <t>TEST test_peasants.produce_enough_land_and_tools()</t>
+    <t>rel_prices</t>
+  </si>
+  <si>
+    <t>TEST test_market._set_prices()</t>
+  </si>
+  <si>
+    <t>reg_prices</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>old_avail</t>
+  </si>
+  <si>
+    <t>diff_prices</t>
+  </si>
+  <si>
+    <t>DERIVATION</t>
+  </si>
+  <si>
+    <t>nondefault</t>
+  </si>
+  <si>
+    <t>-d(ava)</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>max_emps</t>
+  </si>
+  <si>
+    <t>employable</t>
+  </si>
+  <si>
+    <t>wage</t>
+  </si>
+  <si>
+    <t>min_wage</t>
+  </si>
+  <si>
+    <t>land_use</t>
+  </si>
+  <si>
+    <t>total_max_emps</t>
+  </si>
+  <si>
+    <t>total_emps</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>employers_corrected_wage</t>
+  </si>
+  <si>
+    <t>employees_wage_shares</t>
+  </si>
+  <si>
+    <t>ratios</t>
+  </si>
+  <si>
+    <t>employees</t>
   </si>
   <si>
     <t>production</t>
   </si>
   <si>
-    <t>working_peasants</t>
-  </si>
-  <si>
-    <t>need_ratio</t>
-  </si>
-  <si>
-    <t>need_rel</t>
-  </si>
-  <si>
-    <t>avg_prod</t>
-  </si>
-  <si>
-    <t>ideal_ratio</t>
-  </si>
-  <si>
-    <t>peasants</t>
-  </si>
-  <si>
     <t>produced</t>
   </si>
   <si>
-    <t>used</t>
-  </si>
-  <si>
-    <t>tool use</t>
-  </si>
-  <si>
-    <t>TEST test_peasants.produce_not_enough_tools()</t>
-  </si>
-  <si>
-    <t>rel_prices</t>
-  </si>
-  <si>
-    <t>TEST test_market._set_prices()</t>
-  </si>
-  <si>
-    <t>reg_prices</t>
-  </si>
-  <si>
-    <t>land</t>
-  </si>
-  <si>
-    <t>old_avail</t>
-  </si>
-  <si>
-    <t>diff_prices</t>
-  </si>
-  <si>
-    <t>DERIVATION</t>
-  </si>
-  <si>
-    <t>nondefault</t>
-  </si>
-  <si>
-    <t>-d(ava)</t>
+    <t>tools_used</t>
+  </si>
+  <si>
+    <t>tools_usage</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>wage_ratios</t>
+  </si>
+  <si>
+    <t>emps_first_added</t>
+  </si>
+  <si>
+    <t>overemployment</t>
+  </si>
+  <si>
+    <t>emps_second_added</t>
+  </si>
+  <si>
+    <t>emps_second_wages</t>
+  </si>
+  <si>
+    <t>emps_second_total</t>
+  </si>
+  <si>
+    <t>increase_wage?</t>
+  </si>
+  <si>
+    <t>produced_worth</t>
+  </si>
+  <si>
+    <t>used_worth</t>
+  </si>
+  <si>
+    <t>DEFAULT_PRICES</t>
+  </si>
+  <si>
+    <t>profit_share</t>
+  </si>
+  <si>
+    <t>max_wage</t>
+  </si>
+  <si>
+    <t>employer_share</t>
+  </si>
+  <si>
+    <t>employee_share</t>
+  </si>
+  <si>
+    <t>total_produced_share</t>
+  </si>
+  <si>
+    <t>total_used_share</t>
+  </si>
+  <si>
+    <t>raw_prices</t>
+  </si>
+  <si>
+    <t>changed_wage</t>
+  </si>
+  <si>
+    <t>WAGE_CHANGE</t>
+  </si>
+  <si>
+    <t>bottom_checked</t>
+  </si>
+  <si>
+    <t>employer_wage_not_corrected</t>
+  </si>
+  <si>
+    <t>top_checked (NEW_WAGE)</t>
   </si>
 </sst>
 </file>
@@ -217,7 +301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -305,11 +389,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -321,8 +414,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -331,6 +422,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -647,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAE5964-51D9-4F83-BE49-7B6E99C5E897}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
@@ -851,8 +946,8 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>43</v>
+      <c r="A5" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="B5">
         <v>308</v>
@@ -876,23 +971,23 @@
         <v>7</v>
       </c>
       <c r="B6" s="5">
-        <f>SUM(B3,G3,L3)</f>
+        <f t="shared" ref="B6:F7" si="0">SUM(B3,G3,L3)</f>
         <v>310</v>
       </c>
       <c r="C6" s="5">
-        <f>SUM(C3,H3,M3)</f>
+        <f t="shared" si="0"/>
         <v>320</v>
       </c>
       <c r="D6" s="5">
-        <f>SUM(D3,I3,N3)</f>
+        <f t="shared" si="0"/>
         <v>330</v>
       </c>
       <c r="E6" s="5">
-        <f>SUM(E3,J3,O3)</f>
+        <f t="shared" si="0"/>
         <v>340</v>
       </c>
       <c r="F6" s="5">
-        <f>SUM(F3,K3,P3)</f>
+        <f t="shared" si="0"/>
         <v>350</v>
       </c>
       <c r="G6" s="5"/>
@@ -914,23 +1009,23 @@
         <v>5</v>
       </c>
       <c r="B7" s="5">
-        <f>SUM(B4,G4,L4)</f>
+        <f t="shared" si="0"/>
         <v>350</v>
       </c>
       <c r="C7" s="5">
-        <f>SUM(C4,H4,M4)</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="D7" s="5">
-        <f>SUM(D4,I4,N4)</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="E7" s="5">
-        <f>SUM(E4,J4,O4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F7" s="5">
-        <f>SUM(F4,K4,P4)</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="G7" s="5"/>
@@ -968,7 +1063,7 @@
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10">
@@ -986,26 +1081,26 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5">
         <f>IF(B7*B8/B6=0,B8,B7*B8/B6)</f>
         <v>1.1290322580645162</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" ref="C9:F9" si="0">IF(C7*C8/C6=0,C8,C7*C8/C6)</f>
+        <f t="shared" ref="C9:F9" si="1">IF(C7*C8/C6=0,C8,C7*C8/C6)</f>
         <v>0.703125</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1363636363636365</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.3529411764705881E-3</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="G9" s="5"/>
@@ -1028,19 +1123,19 @@
         <v>-2</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:F10" si="1">(C5-C6)</f>
+        <f t="shared" ref="C10:F10" si="2">(C5-C6)</f>
         <v>-20</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="S10" s="6"/>
@@ -1051,19 +1146,19 @@
         <v>0.1353352832366127</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:F11" si="2">EXP(C10)*C8</f>
+        <f t="shared" ref="C11:F11" si="3">EXP(C10)*C8</f>
         <v>3.0917304336578366E-9</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>371.03289775644151</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>371.03289775644151</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.3582814496799134E-2</v>
       </c>
       <c r="S11" s="6"/>
@@ -1077,45 +1172,45 @@
         <v>1.1966998996828226</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" ref="C12:F12" si="3">$J$8*C11+(1-$K$8)*C9</f>
+        <f t="shared" ref="C12:F12" si="4">$J$8*C11+(1-$K$8)*C9</f>
         <v>0.70312500154586521</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>186.65281251458438</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>185.52380181939722</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.5117914072483996</v>
       </c>
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>39</v>
+      <c r="A13" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="B13">
         <f>B9/B8</f>
         <v>1.1290322580645162</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:F13" si="4">C9/C8</f>
+        <f t="shared" ref="C13:F13" si="5">C9/C8</f>
         <v>0.46875</v>
       </c>
       <c r="D13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.45454545454545459</v>
       </c>
       <c r="E13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.9411764705882353E-3</v>
       </c>
       <c r="F13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="S13" s="6"/>
@@ -1418,11 +1513,11 @@
         <v>1</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" ref="C20:D20" si="5">IF(C18&gt;C19,1,0)</f>
+        <f t="shared" ref="C20:D20" si="6">IF(C18&gt;C19,1,0)</f>
         <v>1</v>
       </c>
       <c r="D20" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E20" s="5"/>
@@ -1539,11 +1634,11 @@
         <v>0</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" ref="C23:D23" si="6">(1-C20)*C18/C19</f>
+        <f t="shared" ref="C23:D23" si="7">(1-C20)*C18/C19</f>
         <v>0</v>
       </c>
       <c r="D23" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E23" s="5"/>
@@ -1639,59 +1734,59 @@
         <v>132.85714285714283</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" ref="C25:P25" si="7">C24+C22</f>
+        <f t="shared" ref="C25:P25" si="8">C24+C22</f>
         <v>50</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="G25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>132.85714285714283</v>
       </c>
       <c r="H25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="I25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="J25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="L25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44.285714285714285</v>
       </c>
       <c r="M25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="N25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="O25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="Q25" s="5"/>
@@ -1770,63 +1865,63 @@
         <v>13</v>
       </c>
       <c r="B29" s="5">
-        <f t="shared" ref="B29:P29" si="8">B25</f>
+        <f t="shared" ref="B29:P29" si="9">B25</f>
         <v>132.85714285714283</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="D29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="E29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="G29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>132.85714285714283</v>
       </c>
       <c r="H29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="I29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="J29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="L29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44.285714285714285</v>
       </c>
       <c r="M29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="N29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="O29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="P29" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="Q29" s="5"/>
@@ -1880,11 +1975,11 @@
         <v>27956.446488547648</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" ref="C31:D31" si="9">MAX(C18-C19, 0)</f>
+        <f t="shared" ref="C31:D31" si="10">MAX(C18-C19, 0)</f>
         <v>65515.269552793514</v>
       </c>
       <c r="D31" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3440.2485597721607</v>
       </c>
       <c r="E31" s="5" t="s">
@@ -2051,67 +2146,67 @@
       <c r="S35" s="6"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="12">
         <f>B29+B34</f>
         <v>132.85714285714283</v>
       </c>
-      <c r="C36" s="14">
-        <f t="shared" ref="C36:P36" si="10">C29+C34</f>
+      <c r="C36" s="12">
+        <f t="shared" ref="C36:P36" si="11">C29+C34</f>
         <v>99.040342156044815</v>
       </c>
-      <c r="D36" s="14">
-        <f t="shared" si="10"/>
+      <c r="D36" s="12">
+        <f t="shared" si="11"/>
         <v>101.92506816522392</v>
       </c>
-      <c r="E36" s="14">
-        <f t="shared" si="10"/>
+      <c r="E36" s="12">
+        <f t="shared" si="11"/>
         <v>97.792211711171717</v>
       </c>
-      <c r="F36" s="14">
-        <f t="shared" si="10"/>
+      <c r="F36" s="12">
+        <f t="shared" si="11"/>
         <v>107.69452018358214</v>
       </c>
-      <c r="G36" s="14">
-        <f t="shared" si="10"/>
+      <c r="G36" s="12">
+        <f t="shared" si="11"/>
         <v>132.85714285714283</v>
       </c>
-      <c r="H36" s="14">
-        <f t="shared" si="10"/>
+      <c r="H36" s="12">
+        <f t="shared" si="11"/>
         <v>164.92487919130423</v>
       </c>
-      <c r="I36" s="14">
-        <f t="shared" si="10"/>
+      <c r="I36" s="12">
+        <f t="shared" si="11"/>
         <v>171.68516620255741</v>
       </c>
-      <c r="J36" s="14">
-        <f t="shared" si="10"/>
+      <c r="J36" s="12">
+        <f t="shared" si="11"/>
         <v>229.17372968148311</v>
       </c>
-      <c r="K36" s="14">
-        <f t="shared" si="10"/>
+      <c r="K36" s="12">
+        <f t="shared" si="11"/>
         <v>185.20574022506378</v>
       </c>
-      <c r="L36" s="14">
-        <f t="shared" si="10"/>
+      <c r="L36" s="12">
+        <f t="shared" si="11"/>
         <v>44.285714285714285</v>
       </c>
-      <c r="M36" s="14">
-        <f t="shared" si="10"/>
+      <c r="M36" s="12">
+        <f t="shared" si="11"/>
         <v>56.034778652650992</v>
       </c>
-      <c r="N36" s="14">
-        <f t="shared" si="10"/>
+      <c r="N36" s="12">
+        <f t="shared" si="11"/>
         <v>56.389765632218698</v>
       </c>
-      <c r="O36" s="14">
-        <f t="shared" si="10"/>
+      <c r="O36" s="12">
+        <f t="shared" si="11"/>
         <v>13.034058607345216</v>
       </c>
-      <c r="P36" s="14">
-        <f t="shared" si="10"/>
+      <c r="P36" s="12">
+        <f t="shared" si="11"/>
         <v>57.099739591354108</v>
       </c>
       <c r="Q36" s="7"/>
@@ -2141,7 +2236,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2181,8 +2276,8 @@
       <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>42</v>
+      <c r="G2" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>0</v>
@@ -2199,8 +2294,8 @@
       <c r="L2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="17" t="s">
-        <v>42</v>
+      <c r="M2" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>0</v>
@@ -2217,8 +2312,8 @@
       <c r="R2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="18" t="s">
-        <v>42</v>
+      <c r="S2" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -2323,7 +2418,7 @@
       <c r="L4" s="5">
         <v>50</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="15">
         <v>0</v>
       </c>
       <c r="N4" s="5">
@@ -2349,8 +2444,8 @@
       <c r="V4" s="5"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>43</v>
+      <c r="A5" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="B5" s="5">
         <v>300</v>
@@ -2391,27 +2486,27 @@
         <v>7</v>
       </c>
       <c r="B6" s="5">
-        <f>SUM(B3,H3,N3)</f>
+        <f t="shared" ref="B6:G7" si="0">SUM(B3,H3,N3)</f>
         <v>301</v>
       </c>
       <c r="C6" s="5">
-        <f>SUM(C3,I3,O3)</f>
+        <f t="shared" si="0"/>
         <v>302</v>
       </c>
       <c r="D6" s="5">
-        <f>SUM(D3,J3,P3)</f>
+        <f t="shared" si="0"/>
         <v>303</v>
       </c>
       <c r="E6" s="5">
-        <f>SUM(E3,K3,Q3)</f>
+        <f t="shared" si="0"/>
         <v>304</v>
       </c>
       <c r="F6" s="5">
-        <f>SUM(F3,L3,R3)</f>
+        <f t="shared" si="0"/>
         <v>305</v>
       </c>
       <c r="G6" s="5">
-        <f>SUM(G3,M3,S3)</f>
+        <f t="shared" si="0"/>
         <v>306</v>
       </c>
       <c r="H6" s="5"/>
@@ -2435,27 +2530,27 @@
         <v>5</v>
       </c>
       <c r="B7" s="5">
-        <f>SUM(B4,H4,N4)</f>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="C7" s="5">
-        <f>SUM(C4,I4,O4)</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="D7" s="5">
-        <f>SUM(D4,J4,P4)</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="E7" s="5">
-        <f>SUM(E4,K4,Q4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7" s="5">
-        <f>SUM(F4,L4,R4)</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="G7" s="5">
-        <f>SUM(G4,M4,S4)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="H7" s="5"/>
@@ -2498,7 +2593,7 @@
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10">
@@ -2517,30 +2612,30 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5">
-        <f>IF(B7*B8/B6=0,B8,B7*B8/B6)</f>
+        <f t="shared" ref="B9:G9" si="1">IF(B7*B8/B6=0,B8,B7*B8/B6)</f>
         <v>0.36544850498338871</v>
       </c>
       <c r="C9" s="5">
-        <f>IF(C7*C8/C6=0,C8,C7*C8/C6)</f>
+        <f t="shared" si="1"/>
         <v>0.74503311258278149</v>
       </c>
       <c r="D9" s="5">
-        <f>IF(D7*D8/D6=0,D8,D7*D8/D6)</f>
+        <f t="shared" si="1"/>
         <v>1.2376237623762376</v>
       </c>
       <c r="E9" s="5">
-        <f>IF(E7*E8/E6=0,E8,E7*E8/E6)</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="F9" s="5">
-        <f>IF(F7*F8/F6=0,F8,F7*F8/F6)</f>
+        <f t="shared" si="1"/>
         <v>1.721311475409836</v>
       </c>
       <c r="G9" s="5">
-        <f>IF(G7*G8/G6=0,G8,G7*G8/G6)</f>
+        <f t="shared" si="1"/>
         <v>3.2679738562091503</v>
       </c>
       <c r="H9" s="5"/>
@@ -2559,31 +2654,31 @@
       <c r="U9" s="5"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
-        <v>47</v>
+      <c r="A10" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="B10" s="5">
         <f>(B5-B6)</f>
         <v>-1</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" ref="C10:G10" si="0">(C5-C6)</f>
+        <f t="shared" ref="C10:G10" si="2">(C5-C6)</f>
         <v>-2</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="G10" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-6</v>
       </c>
       <c r="H10" s="5"/>
@@ -2602,31 +2697,31 @@
       <c r="U10" s="5"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>44</v>
+      <c r="A11" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="B11" s="5">
         <f>EXP(B10)*B8</f>
         <v>0.36787944117144233</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" ref="C11:G11" si="1">EXP(C10)*C8</f>
+        <f t="shared" ref="C11:G11" si="3">EXP(C10)*C8</f>
         <v>0.20300292485491905</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>18.472640247326627</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.7957045711476125</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.3582814496799134E-2</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.4787521766663587E-2</v>
       </c>
       <c r="H11" s="5"/>
@@ -2645,7 +2740,7 @@
       <c r="U11" s="5"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="5">
@@ -2653,23 +2748,23 @@
         <v>0.36666397307741549</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" ref="C12:G12" si="2">$K$8*C11+(1-$K$8)*C9</f>
+        <f t="shared" ref="C12:G12" si="4">$K$8*C11+(1-$K$8)*C9</f>
         <v>0.4740180187188503</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.8551320048514324</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.6478522855738067</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.87244714495331754</v>
       </c>
       <c r="G12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.6463806889879069</v>
       </c>
       <c r="H12" s="5"/>
@@ -2688,31 +2783,31 @@
       <c r="U12" s="5"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
-        <v>46</v>
+      <c r="A13" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="B13" s="7">
         <f>B12/B8</f>
         <v>0.36666397307741549</v>
       </c>
       <c r="C13" s="7">
-        <f t="shared" ref="C13:G13" si="3">C12/C8</f>
+        <f t="shared" ref="C13:G13" si="5">C12/C8</f>
         <v>0.31601201247923355</v>
       </c>
       <c r="D13" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.9420528019405729</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.8591409142295228</v>
       </c>
       <c r="F13" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.249270612843805</v>
       </c>
       <c r="G13" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.16463806889879068</v>
       </c>
       <c r="H13" s="7"/>
@@ -3099,199 +3194,199 @@
       <c r="U29" s="5"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="17"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="17"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17"/>
-      <c r="Q33" s="17"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17"/>
-      <c r="Q34" s="17"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
       <c r="U34" s="5"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="17"/>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3299,247 +3394,937 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2335B94E-58D2-46E0-B33A-90F0D910DE22}">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DE598A-8259-4338-8AE6-28C7B9471E26}">
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.3</v>
+      </c>
+      <c r="I2">
+        <v>40</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0.25</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="11">
+      <c r="P2">
+        <v>0.35</v>
+      </c>
+      <c r="R2" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="S2" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19">
         <v>1</v>
       </c>
-      <c r="C3" s="11">
+      <c r="O3" s="19">
         <v>1.5</v>
       </c>
-      <c r="D3" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="15">
+      <c r="P3" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="Q3" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="R3" s="19">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="21">
+        <f>MIN(A2*C2+E2*G2+I2*K2+M2*O2,F4)</f>
+        <v>50</v>
+      </c>
+      <c r="F4" s="21">
+        <f>B2+F2+J2+N2</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="12">
-        <v>1.8</v>
-      </c>
-      <c r="C4" s="12">
+      <c r="G4" s="21"/>
+      <c r="H4">
+        <f>E4/F4</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="19"/>
+      <c r="N4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5">
+        <f>D2</f>
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <f>H2</f>
+        <v>0.3</v>
+      </c>
+      <c r="F5">
+        <f>L2</f>
+        <v>0.25</v>
+      </c>
+      <c r="G5">
+        <f>P2</f>
+        <v>0.35</v>
+      </c>
+      <c r="J5" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" s="19">
+        <v>2</v>
+      </c>
+      <c r="O5" s="20">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="12">
+      <c r="P5" s="19">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="R5" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6">
+        <f>MAX(D2,$R$2)*(B2&gt;0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <f>MAX(H2,$R$2)*(F2&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>MAX(L2,$R$2)*(J2&gt;0)</f>
+        <v>0.3</v>
+      </c>
+      <c r="G6">
+        <f>MAX(P2,$R$2)*(N2&gt;0)</f>
+        <v>0.35</v>
+      </c>
+      <c r="M6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6">
+        <f>N5/SUM($N5:$Q5)</f>
+        <v>0.27586206896551724</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:Q6" si="0">O5/SUM($N5:$Q5)</f>
+        <v>0.20689655172413793</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0.41379310344827586</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>0.10344827586206896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7">
+        <f>A2*C2/$E$4</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>E2*G2/$E$4</f>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f>I2*K2/$E$4</f>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>M2*O2/$E$4</f>
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7">
+        <f>$E$4*N6</f>
+        <v>13.793103448275861</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7:Q7" si="1">$E$4*O6</f>
+        <v>10.344827586206897</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>20.689655172413794</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>5.1724137931034484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8">
+        <f>D6/SUM($D6:$G6)</f>
+        <v>0.43478260869565222</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:G8" si="2">E6/SUM($D6:$G6)</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>0.2608695652173913</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>0.30434782608695654</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="19">
+        <v>1</v>
+      </c>
+      <c r="O8" s="20">
         <v>1.5</v>
       </c>
-      <c r="C5" s="11">
+      <c r="P8" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="Q8" s="19">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9">
+        <f>D8*$E$4</f>
+        <v>21.739130434782609</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:G9" si="3">E8*$E$4</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>13.043478260869565</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>15.217391304347828</v>
+      </c>
+      <c r="H9" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9">
+        <f>N8*N7</f>
+        <v>13.793103448275861</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9:Q9" si="4">O8*O7</f>
+        <v>15.517241379310345</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>14.482758620689655</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="4"/>
+        <v>6.2068965517241379</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <f>MAX(D9-B$2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>MAX(E9-F$2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>MAX(F9-J$2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>MAX(G9-N$2,0)</f>
+        <v>5.2173913043478279</v>
+      </c>
+      <c r="H10">
+        <f>SUM(D10:G10)</f>
+        <v>5.2173913043478279</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="19">
+        <v>0.15</v>
+      </c>
+      <c r="O10">
+        <f>N10</f>
+        <v>0.15</v>
+      </c>
+      <c r="P10" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="Q10">
+        <f>P10</f>
+        <v>0.2</v>
+      </c>
+      <c r="R10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11">
+        <f>D6*(D10=0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:G11" si="5">E6*(E10=0)</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="5"/>
+        <v>0.3</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11">
+        <f>N7*N10</f>
+        <v>2.068965517241379</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ref="O11:Q11" si="6">O7*O10</f>
+        <v>1.5517241379310345</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="6"/>
+        <v>4.1379310344827589</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="6"/>
+        <v>1.0344827586206897</v>
+      </c>
+      <c r="R11">
+        <f>SUM(N11:Q11)</f>
+        <v>8.793103448275863</v>
+      </c>
+      <c r="S11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12">
+        <f>D11/SUM($D11:$G11)*SUM($D10:$G10)</f>
+        <v>3.2608695652173925</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:G12" si="7">E11/SUM($D11:$G11)*SUM($D10:$G10)</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="7"/>
+        <v>1.9565217391304353</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12">
+        <f>N9*N5*N3</f>
+        <v>27.586206896551722</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ref="O12:Q12" si="8">O9*O5*O3</f>
+        <v>34.91379310344827</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="8"/>
+        <v>108.62068965517241</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="8"/>
+        <v>11.637931034482758</v>
+      </c>
+      <c r="S12">
+        <f>SUM(N12:Q12)</f>
+        <v>182.75862068965517</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13">
+        <f>D9-D10+D12</f>
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:G13" si="9">E9-E10+E12</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" t="s">
+        <v>62</v>
+      </c>
+      <c r="R13">
+        <f>R11*R5*R3</f>
+        <v>30.77586206896552</v>
+      </c>
+      <c r="S13">
+        <f>R13</f>
+        <v>30.77586206896552</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14">
+        <f>MAX(D13-B$2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f>MAX(E13-F$2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f>MAX(F13-J$2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f>MAX(G13-N$2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f>SUM(D14:G14)</f>
+        <v>0</v>
+      </c>
+      <c r="R14" t="s">
+        <v>44</v>
+      </c>
+      <c r="S14">
+        <f>S13/S12</f>
+        <v>0.16839622641509436</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="b">
+        <f>D13&lt;$H$4*B2</f>
+        <v>0</v>
+      </c>
+      <c r="E15" t="b">
+        <f>E13&lt;$H$4*F2</f>
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
+        <f>F13&lt;$H$4*J2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <f>B5/B4</f>
-        <v>0.83333333333333326</v>
-      </c>
-      <c r="C6">
-        <f>C5/C4</f>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7">
-        <f>C6/(B6+C6)</f>
-        <v>0.44444444444444442</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8">
-        <f>F3-C8</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="C8">
-        <f>F3*C7</f>
-        <v>26.666666666666664</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9">
-        <f>B8*B3</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="C9">
-        <f>C8*C3</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10">
-        <f>D3*F3</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="G15" t="b">
+        <f>G13&lt;$H$4*N2</f>
+        <v>0</v>
+      </c>
+      <c r="I15" t="str">
+        <f>IF(F15,"P","N")</f>
+        <v>P</v>
+      </c>
+      <c r="R15" t="s">
+        <v>65</v>
+      </c>
+      <c r="S15">
+        <f>1-S14</f>
+        <v>0.83160377358490567</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16">
+        <f>D13/SUM($D13:$G13)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:G16" si="10">E13/SUM($D13:$G13)</f>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="10"/>
+        <v>0.3</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="10"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17">
+        <f>D16*(1-D6)</f>
+        <v>0.25</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:G17" si="11">E16*(1-E6)</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="11"/>
+        <v>0.21</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="11"/>
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18">
+        <f>D7*(1-SUM($D17:$G17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:G18" si="12">E7*(1-SUM($D17:$G17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="12"/>
+        <v>0.41000000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19">
+        <f>D18+D17</f>
+        <v>0.25</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:G19" si="13">E18+E17</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="13"/>
+        <v>0.21</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="13"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20">
+        <f>D16</f>
+        <v>0.5</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20:G20" si="14">E16</f>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="14"/>
+        <v>0.3</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="14"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="11">
-        <v>7.1</v>
-      </c>
-      <c r="C14" s="11">
-        <v>1.5</v>
-      </c>
-      <c r="D14" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="F14" s="15">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="12">
-        <v>1.8</v>
-      </c>
-      <c r="C15" s="12">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="C16" s="11">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17">
-        <f>B16/B15</f>
-        <v>0.83333333333333326</v>
-      </c>
-      <c r="C17">
-        <f>C16/C15</f>
-        <v>1.1333333333333333</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18">
-        <f>C17/(B17+C17)</f>
-        <v>0.57627118644067798</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19">
-        <f>F14-C19</f>
-        <v>25.423728813559322</v>
-      </c>
-      <c r="C19">
-        <f>F14*C18</f>
-        <v>34.576271186440678</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20">
-        <f>B19*B14</f>
-        <v>180.50847457627117</v>
-      </c>
-      <c r="C20">
-        <f>C19*C14</f>
-        <v>51.864406779661017</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21">
-        <f>D14*F14</f>
-        <v>24</v>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>1</v>
+      </c>
+      <c r="M21" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21" t="s">
+        <v>4</v>
+      </c>
+      <c r="P21" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" t="s">
+        <v>2</v>
+      </c>
+      <c r="S21" t="s">
+        <v>3</v>
+      </c>
+      <c r="T21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="22">
+        <f>N9*$D19</f>
+        <v>3.4482758620689653</v>
+      </c>
+      <c r="B22" s="22">
+        <f t="shared" ref="B22:C22" si="15">O9*$D19</f>
+        <v>3.8793103448275863</v>
+      </c>
+      <c r="C22" s="22">
+        <f t="shared" si="15"/>
+        <v>3.6206896551724137</v>
+      </c>
+      <c r="D22" s="22">
+        <f>Q9*$D19</f>
+        <v>1.5517241379310345</v>
+      </c>
+      <c r="E22" s="22">
+        <f>-R11*D20</f>
+        <v>-4.3965517241379315</v>
+      </c>
+      <c r="F22" s="22">
+        <f>N9*$E19</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="22">
+        <f t="shared" ref="G22:I22" si="16">O9*$E19</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="22">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="22">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="22">
+        <f>-R11*E20</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="22">
+        <f>N9*$F19</f>
+        <v>2.8965517241379306</v>
+      </c>
+      <c r="L22" s="22">
+        <f t="shared" ref="L22:N22" si="17">O9*$F19</f>
+        <v>3.2586206896551722</v>
+      </c>
+      <c r="M22" s="22">
+        <f t="shared" si="17"/>
+        <v>3.0413793103448272</v>
+      </c>
+      <c r="N22" s="22">
+        <f t="shared" si="17"/>
+        <v>1.3034482758620689</v>
+      </c>
+      <c r="O22" s="22">
+        <f>-R11*F20</f>
+        <v>-2.6379310344827589</v>
+      </c>
+      <c r="P22" s="22">
+        <f>N9*$G19</f>
+        <v>7.4482758620689653</v>
+      </c>
+      <c r="Q22" s="22">
+        <f t="shared" ref="Q22:S22" si="18">O9*$G19</f>
+        <v>8.3793103448275872</v>
+      </c>
+      <c r="R22" s="22">
+        <f t="shared" si="18"/>
+        <v>7.8206896551724139</v>
+      </c>
+      <c r="S22" s="22">
+        <f t="shared" si="18"/>
+        <v>3.3517241379310345</v>
+      </c>
+      <c r="T22" s="22">
+        <f>-R11*G20</f>
+        <v>-1.7586206896551726</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23">
+        <f>IF(D5&lt;=D6,IF(D15,D6+$J$5,D6-$J$5),D5)</f>
+        <v>0.45</v>
+      </c>
+      <c r="E23">
+        <f>IF(E5&lt;=E6,IF(E15,E6+$J$5,E6-$J$5),E5)</f>
+        <v>0.3</v>
+      </c>
+      <c r="F23">
+        <f>IF(F5&lt;=F6,IF(F15,F6+$J$5,F6-$J$5),F5)</f>
+        <v>0.35</v>
+      </c>
+      <c r="G23">
+        <f>IF(G5&lt;=G6,IF(G15,G6+$J$5,G6-$J$5),G5)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24">
+        <f>MAX(D23,0)</f>
+        <v>0.45</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:G24" si="19">MAX(E23,0)</f>
+        <v>0.3</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="19"/>
+        <v>0.35</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="19"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="22">
+        <f>MIN(D24,$S$15)</f>
+        <v>0.45</v>
+      </c>
+      <c r="E25" s="22">
+        <f t="shared" ref="E25:G25" si="20">MIN(E24,$S$15)</f>
+        <v>0.3</v>
+      </c>
+      <c r="F25" s="22">
+        <f t="shared" si="20"/>
+        <v>0.35</v>
+      </c>
+      <c r="G25" s="22">
+        <f t="shared" si="20"/>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -3554,15 +4339,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010002354AB7EC2EF24DA06C23106C803747" ma:contentTypeVersion="0" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="12ac82f4b51530a6458e69da21eb09e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5464ae2dfd1cba46ef3afe4b411115af">
     <xsd:element name="properties">
@@ -3676,6 +4452,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{356D2B18-87B5-4836-ACC7-8887E858DF72}">
   <ds:schemaRefs>
@@ -3692,14 +4477,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D904AF-352E-4CDF-B047-9525628BC63A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{647172B1-7B3F-4042-89A5-9515C32B35B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3713,4 +4490,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D904AF-352E-4CDF-B047-9525628BC63A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>